<commit_message>
cambios de subir y bajar el valor de la apuesta
</commit_message>
<xml_diff>
--- a/Mejores_estrategias.xlsx
+++ b/Mejores_estrategias.xlsx
@@ -507,7 +507,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
         <v>7</v>
@@ -530,7 +530,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C5" t="n">
         <v>8</v>
@@ -547,10 +547,10 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" t="n">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C6" t="n">
         <v>8</v>
@@ -570,7 +570,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C7" t="n">
         <v>8</v>
@@ -590,7 +590,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C8" t="n">
         <v>8</v>
@@ -607,10 +607,10 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C9" t="n">
         <v>8</v>
@@ -627,10 +627,10 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B10" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C10" t="n">
         <v>8</v>
@@ -650,19 +650,19 @@
         <v>2</v>
       </c>
       <c r="B11" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C11" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D11" t="n">
         <v>200</v>
       </c>
       <c r="E11" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
-        <v>1.25</v>
+        <v>1.375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>